<commit_message>
new generic name (import tableur)
</commit_message>
<xml_diff>
--- a/app/plugins/lesCollections/assets/import_mapping/mapping_lescollections.xlsx
+++ b/app/plugins/lesCollections/assets/import_mapping/mapping_lescollections.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="28040" windowHeight="12960"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162912"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -259,9 +264,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>Feuille de correspondances </t>
-  </si>
-  <si>
     <t>Human readable name of the mapping</t>
   </si>
   <si>
@@ -347,18 +349,44 @@
   </si>
   <si>
     <t>Set to yes to save the data spreadsheet or no to delete it from the server after import</t>
+  </si>
+  <si>
+    <t>Import depuis tableur (XLSX)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -379,13 +407,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -444,7 +477,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -479,7 +512,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -656,7 +689,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -664,52 +697,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="44.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="44.5" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1144,7 +1179,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1158,7 +1193,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -1172,7 +1207,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -1186,7 +1221,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -1200,7 +1235,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -1211,7 +1246,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -1222,7 +1257,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -1233,7 +1268,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -1244,176 +1279,182 @@
         <v>73</v>
       </c>
     </row>
+    <row r="43" spans="1:5">
+      <c r="B43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="B45" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" t="s">
+        <v>81</v>
+      </c>
+      <c r="E46" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" t="s">
+        <v>89</v>
+      </c>
+      <c r="E48" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" t="s">
+        <v>93</v>
+      </c>
+      <c r="E49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>96</v>
+      </c>
+      <c r="E50" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" t="s">
+        <v>99</v>
+      </c>
+      <c r="D51" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" t="s">
+        <v>102</v>
+      </c>
+      <c r="D52" t="s">
+        <v>103</v>
+      </c>
+    </row>
     <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>79</v>
+      </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="C53" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="D53" t="s">
-        <v>76</v>
-      </c>
-      <c r="E53" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="B55" t="s">
-        <v>77</v>
-      </c>
-      <c r="C55" t="s">
-        <v>78</v>
-      </c>
-      <c r="D55" t="s">
-        <v>76</v>
-      </c>
-      <c r="E55" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
         <v>79</v>
       </c>
-      <c r="B56" t="s">
-        <v>80</v>
-      </c>
-      <c r="C56" t="s">
-        <v>81</v>
-      </c>
-      <c r="D56" t="s">
-        <v>82</v>
-      </c>
-      <c r="E56" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" t="s">
-        <v>79</v>
-      </c>
-      <c r="B57" t="s">
-        <v>84</v>
-      </c>
-      <c r="C57" t="s">
-        <v>85</v>
-      </c>
-      <c r="D57" t="s">
-        <v>86</v>
-      </c>
-      <c r="E57" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" t="s">
-        <v>79</v>
-      </c>
-      <c r="B58" t="s">
-        <v>88</v>
-      </c>
-      <c r="C58" t="s">
-        <v>89</v>
-      </c>
-      <c r="D58" t="s">
-        <v>90</v>
-      </c>
-      <c r="E58" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" t="s">
-        <v>79</v>
-      </c>
-      <c r="B59" t="s">
-        <v>92</v>
-      </c>
-      <c r="C59" t="s">
-        <v>93</v>
-      </c>
-      <c r="D59" t="s">
-        <v>94</v>
-      </c>
-      <c r="E59" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" t="s">
-        <v>79</v>
-      </c>
-      <c r="B60" t="s">
-        <v>96</v>
-      </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-      <c r="D60" t="s">
-        <v>97</v>
-      </c>
-      <c r="E60" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" t="s">
-        <v>79</v>
-      </c>
-      <c r="B61" t="s">
-        <v>99</v>
-      </c>
-      <c r="C61" t="s">
-        <v>100</v>
-      </c>
-      <c r="D61" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" t="s">
-        <v>79</v>
-      </c>
-      <c r="B62" t="s">
-        <v>102</v>
-      </c>
-      <c r="C62" t="s">
-        <v>103</v>
-      </c>
-      <c r="D62" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" t="s">
-        <v>79</v>
-      </c>
-      <c r="B63" t="s">
-        <v>105</v>
-      </c>
-      <c r="C63" t="s">
-        <v>106</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="B54" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" t="s">
-        <v>79</v>
-      </c>
-      <c r="B64" t="s">
+      <c r="C54" t="s">
         <v>108</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D54" t="s">
         <v>109</v>
-      </c>
-      <c r="D64" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>